<commit_message>
save 12 01 2026
</commit_message>
<xml_diff>
--- a/4 четверть_21_NPM_Github_storing.xlsx
+++ b/4 четверть_21_NPM_Github_storing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEABC810-15A2-4685-8B58-742DA994C3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFBDF8B-C2B4-4584-AC6B-8F803F97C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="-17745" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="12" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
-  <si>
-    <t>4 четверть_21_NPM_Github_storing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Шаг 1</t>
   </si>
@@ -169,17 +163,37 @@
       <t>yarn</t>
     </r>
   </si>
+  <si>
+    <t>Продолжение Шага 3</t>
+  </si>
+  <si>
+    <t>Шаг 6</t>
+  </si>
+  <si>
+    <t>Шаг 7</t>
+  </si>
+  <si>
+    <t>Модификация чужого проекта для использования в своем</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -273,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -284,37 +298,40 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -598,41 +615,41 @@
   <dimension ref="A2:V46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="8"/>
-    <col min="21" max="21" width="67.77734375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="8"/>
+    <col min="21" max="21" width="67.81640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -651,325 +668,324 @@
       <c r="S2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C3" s="10" t="s">
-        <v>0</v>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C3" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="P3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B13" s="12"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="C18" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="9"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>